<commit_message>
Updated Burndow Chart and Sprint Backlog from sprint 4 Updated Scrum Board and Work Breakdown Structure from the Project
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint 4/Burndown Chart.xlsx
+++ b/Project/Phase 2/Sprint 4/Burndown Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Documents\GanttProject\Project\Phase 2\Sprint 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA3473E-E7B4-45AD-91DA-EA978DD9125E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EBDA89-44D2-438D-A203-CA7341108A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{78BB2992-CB2D-44A3-B61B-FD1B4FD8B255}"/>
   </bookViews>
@@ -703,13 +703,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -807,10 +807,10 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1426,7 +1426,7 @@
   <dimension ref="B3:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1532,13 +1532,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="15"/>
-      <c r="F8" s="14"/>
+      <c r="F8" s="14">
+        <v>1</v>
+      </c>
       <c r="G8" s="14">
         <v>1</v>
       </c>
-      <c r="H8" s="14">
-        <v>1</v>
-      </c>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="11">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="F11" s="20">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G11" s="20">
         <f t="shared" si="0"/>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="H11" s="20">
         <f t="shared" ref="H11" si="1">SUM(H6:H10)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
@@ -1620,11 +1620,11 @@
       </c>
       <c r="F12" s="23">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12" s="23">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" s="23">
         <f t="shared" si="2"/>

</xml_diff>